<commit_message>
counter class and updated sheet of excel
</commit_message>
<xml_diff>
--- a/INOW Automation Data Sheet.xlsx
+++ b/INOW Automation Data Sheet.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\INOW\"/>
     </mc:Choice>
@@ -36,7 +36,7 @@
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7971" uniqueCount="1732">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7975" uniqueCount="1736">
   <si>
     <t>NewBussines</t>
   </si>
@@ -5251,6 +5251,18 @@
   </si>
   <si>
     <t>Underinsured Motorist Bodily Injury*</t>
+  </si>
+  <si>
+    <t>PA0000070-01</t>
+  </si>
+  <si>
+    <t>552.00</t>
+  </si>
+  <si>
+    <t>779.00</t>
+  </si>
+  <si>
+    <t>816.00</t>
   </si>
 </sst>
 </file>
@@ -5839,10 +5851,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.42578125"/>
+    <col min="2" max="2" customWidth="true" width="36.42578125"/>
+    <col min="3" max="3" customWidth="true" width="65.85546875"/>
+    <col min="4" max="4" customWidth="true" width="30.5703125"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -9707,10 +9719,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.42578125" customWidth="1"/>
-    <col min="2" max="2" width="27.28515625" customWidth="1"/>
-    <col min="3" max="3" width="37.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="32.42578125"/>
+    <col min="2" max="2" customWidth="true" width="27.28515625"/>
+    <col min="3" max="3" customWidth="true" width="37.140625"/>
+    <col min="4" max="4" customWidth="true" width="24.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -9804,10 +9816,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="32.7109375" customWidth="1"/>
-    <col min="2" max="2" width="29.140625" customWidth="1"/>
-    <col min="3" max="3" width="38.85546875" customWidth="1"/>
-    <col min="4" max="4" width="15" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="32.7109375"/>
+    <col min="2" max="2" customWidth="true" width="29.140625"/>
+    <col min="3" max="3" customWidth="true" width="38.85546875"/>
+    <col min="4" max="4" customWidth="true" width="15.0"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -9911,8 +9923,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.42578125" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="26.5703125"/>
+    <col min="3" max="3" customWidth="true" width="36.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -9975,8 +9987,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="23.42578125"/>
+    <col min="2" max="2" customWidth="true" width="47.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -10025,10 +10037,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.140625" customWidth="1"/>
-    <col min="2" max="2" width="28.28515625" customWidth="1"/>
-    <col min="3" max="3" width="56" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="33.140625"/>
+    <col min="2" max="2" customWidth="true" width="28.28515625"/>
+    <col min="3" max="3" customWidth="true" width="56.0"/>
+    <col min="4" max="4" customWidth="true" width="17.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -10201,10 +10213,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.85546875" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="41.5703125" customWidth="1"/>
-    <col min="4" max="4" width="24.28515625" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="39.85546875"/>
+    <col min="2" max="2" customWidth="true" width="24.0"/>
+    <col min="3" max="3" customWidth="true" width="41.5703125"/>
+    <col min="4" max="4" customWidth="true" width="24.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -10367,11 +10379,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="64.5703125"/>
+    <col min="4" max="4" customWidth="true" width="27.7109375"/>
+    <col min="5" max="5" customWidth="true" width="15.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -21998,10 +22010,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="27.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.85546875" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="27.7109375"/>
+    <col min="3" max="3" customWidth="true" width="15.85546875"/>
+    <col min="4" max="4" customWidth="true" width="21.28515625"/>
+    <col min="5" max="5" customWidth="true" width="15.0"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:5" x14ac:dyDescent="0.25">
@@ -22023,7 +22035,9 @@
         <v>1706</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
+      <c r="D3" t="s" s="0">
+        <v>1732</v>
+      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.25">
@@ -22031,7 +22045,9 @@
         <v>1714</v>
       </c>
       <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
+      <c r="D4" t="s" s="0">
+        <v>1733</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.25">
@@ -22039,7 +22055,9 @@
         <v>1713</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
+      <c r="D5" t="s" s="0">
+        <v>1734</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.25">
@@ -22047,7 +22065,9 @@
         <v>1711</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="D6" t="s" s="0">
+        <v>1735</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.25">
@@ -22085,10 +22105,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="34.28515625"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="64.5703125"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="22.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="4:7" x14ac:dyDescent="0.25">
@@ -29622,10 +29642,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="5.0"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.140625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375"/>
+    <col min="4" max="4" customWidth="true" width="20.28515625"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -29735,12 +29755,12 @@
       <c r="D11" s="1"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D15" t="s">
+      <c r="D15" t="s" s="0">
         <v>1570</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D16" t="s">
+      <c r="D16" t="s" s="0">
         <v>1670</v>
       </c>
     </row>
@@ -29748,12 +29768,12 @@
       <c r="C17" s="27" t="s">
         <v>1729</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" t="s" s="0">
         <v>1722</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
+      <c r="D18" t="s" s="0">
         <v>1723</v>
       </c>
     </row>
@@ -29825,10 +29845,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.42578125"/>
+    <col min="2" max="2" customWidth="true" width="36.42578125"/>
+    <col min="3" max="3" customWidth="true" width="65.85546875"/>
+    <col min="4" max="4" customWidth="true" width="30.5703125"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -33651,10 +33671,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="64.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="18.85546875"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.28515625"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="64.5703125"/>
+    <col min="4" max="4" customWidth="true" width="33.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -37977,10 +37997,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.42578125"/>
+    <col min="2" max="2" customWidth="true" width="36.42578125"/>
+    <col min="3" max="3" customWidth="true" width="65.85546875"/>
+    <col min="4" max="4" customWidth="true" width="30.5703125"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -41803,10 +41823,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.5703125" customWidth="1"/>
-    <col min="2" max="2" width="21.42578125" customWidth="1"/>
-    <col min="3" max="3" width="46.140625" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.5703125"/>
+    <col min="2" max="2" customWidth="true" width="21.42578125"/>
+    <col min="3" max="3" customWidth="true" width="46.140625"/>
+    <col min="4" max="4" customWidth="true" width="36.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -41928,10 +41948,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.85546875" customWidth="1"/>
-    <col min="2" max="2" width="31.42578125" customWidth="1"/>
-    <col min="3" max="3" width="48" customWidth="1"/>
-    <col min="4" max="4" width="23.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="27.85546875"/>
+    <col min="2" max="2" customWidth="true" width="31.42578125"/>
+    <col min="3" max="3" customWidth="true" width="48.0"/>
+    <col min="4" max="4" customWidth="true" width="23.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -42069,10 +42089,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="51" customWidth="1"/>
-    <col min="2" max="2" width="49" customWidth="1"/>
-    <col min="3" max="3" width="40.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.85546875" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="51.0"/>
+    <col min="2" max="2" customWidth="true" width="49.0"/>
+    <col min="3" max="3" customWidth="true" width="40.28515625"/>
+    <col min="4" max="4" customWidth="true" width="25.85546875"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -42214,10 +42234,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.42578125" customWidth="1"/>
-    <col min="2" max="2" width="33.7109375" customWidth="1"/>
-    <col min="3" max="3" width="40.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.42578125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="31.42578125"/>
+    <col min="2" max="2" customWidth="true" width="33.7109375"/>
+    <col min="3" max="3" customWidth="true" width="40.5703125"/>
+    <col min="4" max="4" customWidth="true" width="33.42578125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -42313,10 +42333,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" customWidth="1"/>
-    <col min="2" max="2" width="29.42578125" customWidth="1"/>
-    <col min="3" max="3" width="38.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="33.5703125"/>
+    <col min="2" max="2" customWidth="true" width="29.42578125"/>
+    <col min="3" max="3" customWidth="true" width="38.42578125"/>
+    <col min="4" max="4" customWidth="true" width="12.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -42424,10 +42444,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.42578125" customWidth="1"/>
-    <col min="3" max="3" width="65.85546875" customWidth="1"/>
-    <col min="4" max="4" width="30.5703125" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="24.42578125"/>
+    <col min="2" max="2" customWidth="true" width="36.42578125"/>
+    <col min="3" max="3" customWidth="true" width="65.85546875"/>
+    <col min="4" max="4" customWidth="true" width="30.5703125"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>